<commit_message>
add new species by CRZ and more
</commit_message>
<xml_diff>
--- a/inst/newtaxa_occurrences/raw/occurrences_novedades_tax.xlsx
+++ b/inst/newtaxa_occurrences/raw/occurrences_novedades_tax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNI\4. DOCTORADO\99. OTROS\2021_10_07 AFLIBER 2.0\AFLIBER_update\inst\newtaxa_occurrences\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC5421D-93E2-4F73-A8D4-381DB7F67B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBA317C-A964-4D8D-85C6-A449AA08D9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{22E89CF6-412E-4101-9F04-7902DEF2EDAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22E89CF6-412E-4101-9F04-7902DEF2EDAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>UJA</author>
   </authors>
   <commentList>
-    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{15E69A07-4261-4A06-B32B-2A4F706C2788}">
+    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{15E69A07-4261-4A06-B32B-2A4F706C2788}">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="120">
   <si>
     <t>Species</t>
   </si>
@@ -837,6 +837,39 @@
   </si>
   <si>
     <t>newtaxa_occurrences</t>
+  </si>
+  <si>
+    <t>Digitaria debilis</t>
+  </si>
+  <si>
+    <t>29TNE15</t>
+  </si>
+  <si>
+    <t>29TNG22</t>
+  </si>
+  <si>
+    <t>29TNF37</t>
+  </si>
+  <si>
+    <t>29TNE45</t>
+  </si>
+  <si>
+    <t>29TNG40</t>
+  </si>
+  <si>
+    <t>29SQA29</t>
+  </si>
+  <si>
+    <t>29SPB51</t>
+  </si>
+  <si>
+    <t>29SQD27</t>
+  </si>
+  <si>
+    <t>30TTK73</t>
+  </si>
+  <si>
+    <t>Flora-On: Flora de Portugal Interactiva. Sociedade Portuguesa de Botânica. www.flora-on.pt. Last accessed February, 2025.</t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A7FFF5-FBB4-4A11-8781-7BABF3FCEBB3}">
-  <dimension ref="A2:D94"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,18 +1289,32 @@
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,7 +1322,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1288,8 +1335,8 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1302,8 +1349,8 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1317,7 +1364,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1331,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1345,7 +1392,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1359,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1373,7 +1420,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1387,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1398,13 +1445,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -1415,7 +1462,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -1429,7 +1476,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1443,7 +1490,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1457,7 +1504,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -1471,7 +1518,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -1485,7 +1532,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -1499,7 +1546,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -1513,7 +1560,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -1527,7 +1574,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -1541,7 +1588,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -1555,7 +1602,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -1569,7 +1616,7 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -1583,7 +1630,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
@@ -1597,7 +1644,7 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
@@ -1611,7 +1658,7 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
@@ -1625,7 +1672,7 @@
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
@@ -1639,7 +1686,7 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -1653,7 +1700,7 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
@@ -1664,27 +1711,27 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D32" t="s">
         <v>41</v>
@@ -1695,7 +1742,7 @@
         <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>44</v>
@@ -1709,7 +1756,7 @@
         <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>44</v>
@@ -1723,7 +1770,7 @@
         <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>44</v>
@@ -1734,13 +1781,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
         <v>41</v>
@@ -1751,7 +1798,7 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>47</v>
@@ -1762,13 +1809,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D38" t="s">
         <v>41</v>
@@ -1776,13 +1823,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1793,7 +1840,7 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>54</v>
@@ -1807,7 +1854,7 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>54</v>
@@ -1821,7 +1868,7 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>54</v>
@@ -1835,7 +1882,7 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>54</v>
@@ -1846,13 +1893,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D44" t="s">
         <v>41</v>
@@ -1860,13 +1907,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D45" t="s">
         <v>41</v>
@@ -1877,7 +1924,7 @@
         <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>62</v>
@@ -1891,7 +1938,7 @@
         <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>62</v>
@@ -1902,13 +1949,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
         <v>41</v>
@@ -1919,7 +1966,7 @@
         <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>70</v>
@@ -1933,7 +1980,7 @@
         <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>70</v>
@@ -1947,7 +1994,7 @@
         <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>70</v>
@@ -1961,7 +2008,7 @@
         <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>70</v>
@@ -1975,7 +2022,7 @@
         <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>70</v>
@@ -1986,13 +2033,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
         <v>41</v>
@@ -2003,7 +2050,7 @@
         <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>75</v>
@@ -2014,13 +2061,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
         <v>41</v>
@@ -2031,7 +2078,7 @@
         <v>79</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>62</v>
@@ -2045,7 +2092,7 @@
         <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>62</v>
@@ -2056,13 +2103,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D59" t="s">
         <v>41</v>
@@ -2073,7 +2120,7 @@
         <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>83</v>
@@ -2084,13 +2131,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D61" t="s">
         <v>41</v>
@@ -2101,7 +2148,7 @@
         <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>87</v>
@@ -2112,13 +2159,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
       </c>
       <c r="D63" t="s">
         <v>41</v>
@@ -2126,13 +2173,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D64" t="s">
         <v>41</v>
@@ -2140,13 +2187,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D65" t="s">
         <v>41</v>
@@ -2154,13 +2201,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>92</v>
+        <v>22</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
       </c>
       <c r="D66" t="s">
         <v>41</v>
@@ -2171,7 +2218,7 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C67" t="s">
         <v>19</v>
@@ -2185,7 +2232,7 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C68" t="s">
         <v>19</v>
@@ -2199,7 +2246,7 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C69" t="s">
         <v>19</v>
@@ -2213,7 +2260,7 @@
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C70" t="s">
         <v>19</v>
@@ -2227,7 +2274,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C71" t="s">
         <v>19</v>
@@ -2241,7 +2288,7 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C72" t="s">
         <v>19</v>
@@ -2255,7 +2302,7 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
         <v>19</v>
@@ -2269,7 +2316,7 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="C74" t="s">
         <v>19</v>
@@ -2283,7 +2330,7 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
         <v>19</v>
@@ -2297,7 +2344,7 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s">
         <v>19</v>
@@ -2311,7 +2358,7 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C77" t="s">
         <v>19</v>
@@ -2325,7 +2372,7 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C78" t="s">
         <v>19</v>
@@ -2339,7 +2386,7 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="C79" t="s">
         <v>19</v>
@@ -2353,7 +2400,7 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="C80" t="s">
         <v>19</v>
@@ -2367,7 +2414,7 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C81" t="s">
         <v>19</v>
@@ -2381,7 +2428,7 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C82" t="s">
         <v>19</v>
@@ -2395,7 +2442,7 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C83" t="s">
         <v>19</v>
@@ -2409,7 +2456,7 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
         <v>19</v>
@@ -2420,30 +2467,30 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C85" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="D85" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B86" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="C86" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D86" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2451,7 +2498,7 @@
         <v>98</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C87" t="s">
         <v>107</v>
@@ -2465,7 +2512,7 @@
         <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C88" t="s">
         <v>107</v>
@@ -2479,7 +2526,7 @@
         <v>98</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C89" t="s">
         <v>107</v>
@@ -2493,7 +2540,7 @@
         <v>98</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C90" t="s">
         <v>107</v>
@@ -2507,7 +2554,7 @@
         <v>98</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C91" t="s">
         <v>107</v>
@@ -2521,7 +2568,7 @@
         <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
         <v>107</v>
@@ -2535,7 +2582,7 @@
         <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
         <v>107</v>
@@ -2546,16 +2593,116 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C94" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D94" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>109</v>
+      </c>
+      <c r="B95" t="s">
+        <v>111</v>
+      </c>
+      <c r="C95" t="s">
+        <v>119</v>
+      </c>
+      <c r="D95" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" t="s">
+        <v>112</v>
+      </c>
+      <c r="C96" t="s">
+        <v>119</v>
+      </c>
+      <c r="D96" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97" t="s">
+        <v>113</v>
+      </c>
+      <c r="C97" t="s">
+        <v>119</v>
+      </c>
+      <c r="D97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" t="s">
+        <v>114</v>
+      </c>
+      <c r="C98" t="s">
+        <v>119</v>
+      </c>
+      <c r="D98" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>109</v>
+      </c>
+      <c r="B99" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100" t="s">
+        <v>116</v>
+      </c>
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101" t="s">
+        <v>117</v>
+      </c>
+      <c r="C101" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>109</v>
+      </c>
+      <c r="B102" t="s">
+        <v>118</v>
+      </c>
+      <c r="C102" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>